<commit_message>
zmena verzie dependency log4j lebo nesiel export
</commit_message>
<xml_diff>
--- a/src/FinalApp/exports/Inventory.xlsx
+++ b/src/FinalApp/exports/Inventory.xlsx
@@ -6,13 +6,13 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Inventúra 2023-12-23" r:id="rId3" sheetId="1"/>
+    <sheet name="Inventúra 2024-01-15" r:id="rId3" sheetId="1"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>Pozícia</t>
   </si>
@@ -29,22 +29,25 @@
     <t>A0001</t>
   </si>
   <si>
-    <t>001</t>
+    <t>2000</t>
   </si>
   <si>
-    <t>Motor 100</t>
+    <t>Test material</t>
   </si>
   <si>
-    <t>2</t>
+    <t>5</t>
+  </si>
+  <si>
+    <t>2766</t>
+  </si>
+  <si>
+    <t>ds</t>
+  </si>
+  <si>
+    <t>8</t>
   </si>
   <si>
     <t>A0002</t>
-  </si>
-  <si>
-    <t>002</t>
-  </si>
-  <si>
-    <t>Skrina</t>
   </si>
 </sst>
 </file>
@@ -89,7 +92,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -125,15 +128,29 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="B3" t="s" s="0">
+      <c r="C3" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="C3" t="s" s="0">
+      <c r="D3" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="D3" t="s" s="0">
+    </row>
+    <row r="4">
+      <c r="A4" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="D4" t="s" s="0">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
odskúšala som zmenenie vzhľadu buttonov
</commit_message>
<xml_diff>
--- a/src/FinalApp/exports/Inventory.xlsx
+++ b/src/FinalApp/exports/Inventory.xlsx
@@ -6,13 +6,13 @@
     <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Inventúra 2024-01-15" r:id="rId3" sheetId="1"/>
+    <sheet name="Inventúra 2024-01-24" r:id="rId3" sheetId="1"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="33">
   <si>
     <t>Pozícia</t>
   </si>
@@ -26,28 +26,91 @@
     <t>Počet</t>
   </si>
   <si>
-    <t>A0001</t>
+    <t>A0115</t>
+  </si>
+  <si>
+    <t>2005</t>
+  </si>
+  <si>
+    <t>lampa</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>A0475</t>
   </si>
   <si>
     <t>2000</t>
   </si>
   <si>
-    <t>Test material</t>
+    <t>macka</t>
+  </si>
+  <si>
+    <t>kacka</t>
   </si>
   <si>
     <t>5</t>
   </si>
   <si>
-    <t>2766</t>
-  </si>
-  <si>
-    <t>ds</t>
+    <t>2006</t>
+  </si>
+  <si>
+    <t>kalkulacka</t>
+  </si>
+  <si>
+    <t>srob</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>2001</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>lopata</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>A0015</t>
+  </si>
+  <si>
+    <t>2004</t>
+  </si>
+  <si>
+    <t>kvety</t>
+  </si>
+  <si>
+    <t>mobil</t>
+  </si>
+  <si>
+    <t>paprad</t>
+  </si>
+  <si>
+    <t>lopta</t>
+  </si>
+  <si>
+    <t>okno</t>
+  </si>
+  <si>
+    <t>lava</t>
   </si>
   <si>
     <t>8</t>
   </si>
   <si>
-    <t>A0002</t>
+    <t>C0640</t>
+  </si>
+  <si>
+    <t>2003</t>
+  </si>
+  <si>
+    <t>makrela</t>
   </si>
 </sst>
 </file>
@@ -92,7 +155,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -128,30 +191,198 @@
     </row>
     <row r="3">
       <c r="A3" t="s" s="0">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s" s="0">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s" s="0">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="B4" t="s" s="0">
-        <v>5</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>6</v>
-      </c>
       <c r="D4" t="s" s="0">
-        <v>7</v>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s" s="0">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s" s="0">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s" s="0">
+        <v>11</v>
+      </c>
+      <c r="D7" t="s" s="0">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="D8" t="s" s="0">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="B9" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s" s="0">
+        <v>23</v>
+      </c>
+      <c r="D9" t="s" s="0">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="B10" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="C10" t="s" s="0">
+        <v>24</v>
+      </c>
+      <c r="D10" t="s" s="0">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="D11" t="s" s="0">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="C12" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="D12" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s" s="0">
+        <v>27</v>
+      </c>
+      <c r="D13" t="s" s="0">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="B14" t="s" s="0">
+        <v>22</v>
+      </c>
+      <c r="C14" t="s" s="0">
+        <v>28</v>
+      </c>
+      <c r="D14" t="s" s="0">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="B15" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="C15" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="D15" t="s" s="0">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s" s="0">
+        <v>30</v>
+      </c>
+      <c r="B16" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="C16" t="s" s="0">
+        <v>26</v>
+      </c>
+      <c r="D16" t="s" s="0">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>